<commit_message>
archivos agragando fecha de descrip...
</commit_message>
<xml_diff>
--- a/src/main/webapp/archivos/LC1010-10 Formato de planilla industrial.xlsx
+++ b/src/main/webapp/archivos/LC1010-10 Formato de planilla industrial.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="19260" windowHeight="5535" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Descripción por campo'!$A$1:$D$44</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>Nº</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>Información constante del dependiente</t>
+  </si>
+  <si>
+    <t>dia/mes/año Ejemplo: 11/09/2001</t>
   </si>
 </sst>
 </file>
@@ -600,25 +603,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -986,23 +989,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="45.75" thickBot="1">
+    <row r="1" spans="1:43" ht="32.25" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1191,15 +1194,15 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" thickBot="1">
@@ -1212,7 +1215,7 @@
       <c r="C1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1226,7 +1229,7 @@
       <c r="C2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="11">
@@ -1238,7 +1241,7 @@
       <c r="C3" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1252,7 +1255,7 @@
       <c r="C4" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="11">
@@ -1264,7 +1267,7 @@
       <c r="C5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" ht="25.5">
       <c r="A6" s="11">
@@ -1276,7 +1279,7 @@
       <c r="C6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="25.5">
       <c r="A7" s="11">
@@ -1288,7 +1291,7 @@
       <c r="C7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1299,10 +1302,10 @@
       <c r="B8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11">
@@ -1311,8 +1314,8 @@
       <c r="B9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11">
@@ -1321,8 +1324,8 @@
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11">
@@ -1331,8 +1334,8 @@
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="25.5">
       <c r="A12" s="11">
@@ -1341,8 +1344,8 @@
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1356,7 +1359,7 @@
       <c r="C13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="26" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1368,7 +1371,9 @@
         <v>12</v>
       </c>
       <c r="C14" s="23"/>
-      <c r="D14" s="29"/>
+      <c r="D14" s="27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11">
@@ -1380,7 +1385,7 @@
       <c r="C15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11">
@@ -1392,7 +1397,7 @@
       <c r="C16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" ht="51">
       <c r="A17" s="11">
@@ -1404,7 +1409,7 @@
       <c r="C17" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11">
@@ -1416,7 +1421,7 @@
       <c r="C18" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="26" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1430,7 +1435,9 @@
       <c r="C19" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="38.25">
       <c r="A20" s="11">
@@ -1442,7 +1449,7 @@
       <c r="C20" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="26" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1456,7 +1463,7 @@
       <c r="C21" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11">
@@ -1468,7 +1475,7 @@
       <c r="C22" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="27"/>
     </row>
     <row r="23" spans="1:4" ht="25.5">
       <c r="A23" s="11">
@@ -1480,7 +1487,7 @@
       <c r="C23" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="26" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1494,7 +1501,7 @@
       <c r="C24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11">
@@ -1506,9 +1513,9 @@
       <c r="C25" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="29"/>
-    </row>
-    <row r="26" spans="1:4" ht="25.5">
+      <c r="D25" s="27"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -1518,9 +1525,9 @@
       <c r="C26" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="29"/>
-    </row>
-    <row r="27" spans="1:4" ht="25.5">
+      <c r="D26" s="27"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -1530,7 +1537,7 @@
       <c r="C27" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="11">
@@ -1540,7 +1547,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="23"/>
-      <c r="D28" s="29"/>
+      <c r="D28" s="27"/>
     </row>
     <row r="29" spans="1:4" ht="25.5">
       <c r="A29" s="11">
@@ -1552,7 +1559,7 @@
       <c r="C29" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:4" ht="25.5">
       <c r="A30" s="11">
@@ -1564,7 +1571,7 @@
       <c r="C30" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:4" ht="25.5">
       <c r="A31" s="11">
@@ -1576,7 +1583,7 @@
       <c r="C31" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:4" ht="25.5">
       <c r="A32" s="11">
@@ -1588,7 +1595,7 @@
       <c r="C32" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:4" ht="25.5">
       <c r="A33" s="11">
@@ -1600,7 +1607,7 @@
       <c r="C33" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="27"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="11">
@@ -1610,7 +1617,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="23"/>
-      <c r="D34" s="29"/>
+      <c r="D34" s="27"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="11">
@@ -1620,7 +1627,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="23"/>
-      <c r="D35" s="29"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="11">
@@ -1630,7 +1637,7 @@
         <v>42</v>
       </c>
       <c r="C36" s="23"/>
-      <c r="D36" s="29"/>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="11">
@@ -1640,7 +1647,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="23"/>
-      <c r="D37" s="29"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="11">
@@ -1652,7 +1659,7 @@
       <c r="C38" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="11">
@@ -1662,7 +1669,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="23"/>
-      <c r="D39" s="29"/>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="11">
@@ -1672,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="23"/>
-      <c r="D40" s="29"/>
+      <c r="D40" s="27"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="11">
@@ -1682,7 +1689,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="23"/>
-      <c r="D41" s="29"/>
+      <c r="D41" s="27"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="11">
@@ -1694,7 +1701,7 @@
       <c r="C42" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="29"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="11">
@@ -1706,7 +1713,7 @@
       <c r="C43" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="29"/>
+      <c r="D43" s="27"/>
     </row>
     <row r="44" spans="1:4" ht="39" thickBot="1">
       <c r="A44" s="12">
@@ -1716,7 +1723,7 @@
         <v>41</v>
       </c>
       <c r="C44" s="13"/>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="28" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>